<commit_message>
Add final results and visualiztion of CIFAR-100
</commit_message>
<xml_diff>
--- a/dongha/result/CIFAR_Result.xlsx
+++ b/dongha/result/CIFAR_Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310CB64F-9D21-4586-8EB4-B7C2C726D892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD330869-2B89-46D8-91A4-9EB3EC7DFBED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-1930" windowWidth="25820" windowHeight="15620" xr2:uid="{F1D9A045-ECE6-4DB9-8F9E-A263193934F9}"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15400" xr2:uid="{F1D9A045-ECE6-4DB9-8F9E-A263193934F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -488,28 +488,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{529EDAAB-ADDB-4014-83BC-7A428929F350}">
   <dimension ref="E6:Q33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="B20" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="6" max="6" width="4" customWidth="1"/>
-    <col min="7" max="7" width="16.625" customWidth="1"/>
+    <col min="7" max="7" width="16.58203125" customWidth="1"/>
     <col min="8" max="15" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:17" x14ac:dyDescent="0.45">
       <c r="E6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="5:17" x14ac:dyDescent="0.45">
       <c r="E7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="5:17" x14ac:dyDescent="0.45">
       <c r="E8" t="s">
         <v>8</v>
       </c>
@@ -532,7 +532,7 @@
       <c r="P8" s="1"/>
       <c r="Q8" s="1"/>
     </row>
-    <row r="9" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="5:17" x14ac:dyDescent="0.45">
       <c r="E9" t="s">
         <v>9</v>
       </c>
@@ -561,7 +561,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="5:17" x14ac:dyDescent="0.45">
       <c r="G10" t="s">
         <v>11</v>
       </c>
@@ -590,7 +590,7 @@
         <v>0.71449999999999902</v>
       </c>
     </row>
-    <row r="11" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="5:17" x14ac:dyDescent="0.45">
       <c r="G11" t="s">
         <v>12</v>
       </c>
@@ -619,7 +619,7 @@
         <v>0.67699999999999905</v>
       </c>
     </row>
-    <row r="12" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="5:17" x14ac:dyDescent="0.45">
       <c r="G12" t="s">
         <v>10</v>
       </c>
@@ -648,7 +648,7 @@
         <v>0.80549999999999999</v>
       </c>
     </row>
-    <row r="13" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:17" x14ac:dyDescent="0.45">
       <c r="G13" t="s">
         <v>13</v>
       </c>
@@ -677,7 +677,7 @@
         <v>0.70809999999999995</v>
       </c>
     </row>
-    <row r="14" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="14" spans="5:17" x14ac:dyDescent="0.45">
       <c r="G14" t="s">
         <v>14</v>
       </c>
@@ -706,7 +706,7 @@
         <v>0.70840000000000003</v>
       </c>
     </row>
-    <row r="15" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:17" x14ac:dyDescent="0.45">
       <c r="G15" t="s">
         <v>15</v>
       </c>
@@ -735,7 +735,7 @@
         <v>0.67330000000000001</v>
       </c>
     </row>
-    <row r="16" spans="5:17" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:17" x14ac:dyDescent="0.45">
       <c r="G16" t="s">
         <v>16</v>
       </c>
@@ -764,7 +764,7 @@
         <v>0.76700000000000002</v>
       </c>
     </row>
-    <row r="17" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G17" t="s">
         <v>17</v>
       </c>
@@ -793,7 +793,7 @@
         <v>0.78620000000000001</v>
       </c>
     </row>
-    <row r="18" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G18" t="s">
         <v>18</v>
       </c>
@@ -822,7 +822,7 @@
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="19" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G19" t="s">
         <v>19</v>
       </c>
@@ -851,7 +851,7 @@
         <v>0.77900000000000003</v>
       </c>
     </row>
-    <row r="22" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:15" x14ac:dyDescent="0.45">
       <c r="E22" t="s">
         <v>20</v>
       </c>
@@ -872,7 +872,7 @@
       </c>
       <c r="O22" s="1"/>
     </row>
-    <row r="23" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:15" x14ac:dyDescent="0.45">
       <c r="H23" t="s">
         <v>0</v>
       </c>
@@ -898,7 +898,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G24" t="s">
         <v>11</v>
       </c>
@@ -927,7 +927,7 @@
         <v>0.4158</v>
       </c>
     </row>
-    <row r="25" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G25" t="s">
         <v>12</v>
       </c>
@@ -956,7 +956,7 @@
         <v>0.33560000000000001</v>
       </c>
     </row>
-    <row r="26" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G26" t="s">
         <v>10</v>
       </c>
@@ -985,7 +985,7 @@
         <v>0.47920000000000001</v>
       </c>
     </row>
-    <row r="27" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G27" t="s">
         <v>13</v>
       </c>
@@ -1014,50 +1014,183 @@
         <v>0.37880000000000003</v>
       </c>
     </row>
-    <row r="28" spans="5:15" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G28" t="s">
         <v>14</v>
       </c>
       <c r="H28">
         <v>0.39024527828986999</v>
       </c>
+      <c r="I28">
+        <v>0.38233298562824503</v>
+      </c>
       <c r="J28">
         <v>0.39229999999999998</v>
       </c>
+      <c r="K28">
+        <v>0.38400000000000001</v>
+      </c>
       <c r="L28">
         <v>0.41095791626345202</v>
       </c>
+      <c r="M28">
+        <v>0.38601445988060701</v>
+      </c>
       <c r="N28">
         <v>0.39229999999999998</v>
       </c>
-    </row>
-    <row r="29" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="O28">
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G29" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="H29">
+        <v>0.35498814025467101</v>
+      </c>
+      <c r="I29">
+        <v>0.35090711441950301</v>
+      </c>
+      <c r="J29">
+        <v>0.35980000000000001</v>
+      </c>
+      <c r="K29">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="L29">
+        <v>0.36361516869767802</v>
+      </c>
+      <c r="M29">
+        <v>0.35917234233016798</v>
+      </c>
+      <c r="N29">
+        <v>0.35980000000000001</v>
+      </c>
+      <c r="O29">
+        <v>0.35299999999999998</v>
+      </c>
+    </row>
+    <row r="30" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G30" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="H30">
+        <v>0.43264137058639701</v>
+      </c>
+      <c r="I30">
+        <v>0.42309702160504398</v>
+      </c>
+      <c r="J30">
+        <v>0.43240000000000001</v>
+      </c>
+      <c r="K30">
+        <v>0.42809999999999998</v>
+      </c>
+      <c r="L30">
+        <v>0.45040682258230003</v>
+      </c>
+      <c r="M30">
+        <v>0.42833275179350699</v>
+      </c>
+      <c r="N30">
+        <v>0.43240000000000001</v>
+      </c>
+      <c r="O30">
+        <v>0.42809999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G31" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="32" spans="5:15" x14ac:dyDescent="0.3">
+      <c r="H31">
+        <v>0.43179732631295198</v>
+      </c>
+      <c r="I31">
+        <v>0.399253818183811</v>
+      </c>
+      <c r="J31">
+        <v>0.43230000000000002</v>
+      </c>
+      <c r="K31">
+        <v>0.40510000000000002</v>
+      </c>
+      <c r="L31">
+        <v>0.44802092935657301</v>
+      </c>
+      <c r="M31">
+        <v>0.40223655995415403</v>
+      </c>
+      <c r="N31">
+        <v>0.43230000000000002</v>
+      </c>
+      <c r="O31">
+        <v>0.40510000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="5:15" x14ac:dyDescent="0.45">
       <c r="G32" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
+      <c r="H32">
+        <v>0.43692017285649998</v>
+      </c>
+      <c r="I32">
+        <v>0.36947713033653101</v>
+      </c>
+      <c r="J32">
+        <v>0.44040000000000001</v>
+      </c>
+      <c r="K32">
+        <v>0.37580000000000002</v>
+      </c>
+      <c r="L32">
+        <v>0.445718087135696</v>
+      </c>
+      <c r="M32">
+        <v>0.376053887413137</v>
+      </c>
+      <c r="N32">
+        <v>0.44040000000000001</v>
+      </c>
+      <c r="O32">
+        <v>0.37580000000000002</v>
+      </c>
+    </row>
+    <row r="33" spans="7:15" x14ac:dyDescent="0.45">
       <c r="G33" t="s">
         <v>19</v>
       </c>
+      <c r="H33">
+        <v>0.45003995025529597</v>
+      </c>
+      <c r="I33">
+        <v>0.31733321055350699</v>
+      </c>
+      <c r="J33">
+        <v>0.44669999999999999</v>
+      </c>
+      <c r="K33">
+        <v>0.3387</v>
+      </c>
+      <c r="L33">
+        <v>0.463360608267949</v>
+      </c>
+      <c r="M33">
+        <v>0.325901286080852</v>
+      </c>
+      <c r="N33">
+        <v>0.44669999999999999</v>
+      </c>
+      <c r="O33">
+        <v>0.3387</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="P8:Q8"/>
     <mergeCell ref="H22:I22"/>
     <mergeCell ref="J22:K22"/>
     <mergeCell ref="L22:M22"/>
@@ -1066,7 +1199,6 @@
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="N8:O8"/>
-    <mergeCell ref="P8:Q8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>